<commit_message>
ajusta configurações para demais bases
</commit_message>
<xml_diff>
--- a/src/info/aquis_censo_gestor_cols.xlsx
+++ b/src/info/aquis_censo_gestor_cols.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro.forli\PycharmProjects\curso-ciencia-dados\src\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFFE4708-A14E-4797-B89A-510AE870A5E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDCFF8D-779D-433A-BA72-66B0B256E392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{48C7DDBA-442F-4222-8A07-8EDC411B5A7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{48C7DDBA-442F-4222-8A07-8EDC411B5A7F}"/>
   </bookViews>
   <sheets>
     <sheet name="dtype" sheetId="14" r:id="rId1"/>
@@ -863,7 +863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70D7738B-264F-484F-BE6D-FD3693129414}">
   <dimension ref="A1:C199"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2219,7 +2219,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F00CDFD-68EC-4FE5-BDA4-86E9DB42A085}">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2327,7 +2329,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2956,7 +2958,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3258CC0-ADA6-4507-AB64-D90060B3088F}">
   <dimension ref="A1:B84"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3064,7 +3068,7 @@
         <v>10</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>